<commit_message>
Small fixes for triangle input
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Nome</t>
   </si>
@@ -47,13 +47,16 @@
     <t>% de acertos</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>00:00:21</t>
-  </si>
-  <si>
-    <t>00:00:12</t>
+    <t>Teste2</t>
+  </si>
+  <si>
+    <t>12/12/2012</t>
+  </si>
+  <si>
+    <t>00:00:11</t>
+  </si>
+  <si>
+    <t>00:00:08</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3">
         <v>500</v>
@@ -538,13 +541,13 @@
         <v>100</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J3" s="4">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3">
         <v>500</v>
@@ -649,19 +652,19 @@
         <v>600</v>
       </c>
       <c r="F3" s="5">
+        <v>100</v>
+      </c>
+      <c r="G3" s="5">
         <v>50</v>
       </c>
-      <c r="G3" s="5">
-        <v>15</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J3" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean Coding Oh my god
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -47,16 +47,16 @@
     <t>% de acertos</t>
   </si>
   <si>
-    <t>Teste2</t>
-  </si>
-  <si>
-    <t>12/12/2012</t>
-  </si>
-  <si>
-    <t>00:00:11</t>
-  </si>
-  <si>
-    <t>00:00:08</t>
+    <t>Rosa</t>
+  </si>
+  <si>
+    <t>HOJE</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>00:00:10</t>
   </si>
 </sst>
 </file>

</xml_diff>